<commit_message>
harmonised offset data (04.02.2026 version)
</commit_message>
<xml_diff>
--- a/nba2k_editor/Offsets/ImportJerseys.xlsx
+++ b/nba2k_editor/Offsets/ImportJerseys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jersey Vitals" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Jersey Colors" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Jersey Vitals" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Jersey Colors" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,16 +18,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -38,7 +35,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -46,21 +43,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -435,137 +423,137 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>COLOR_LUMINANCE_LEVEL</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Edition Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>EDITION_CRC32B</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>FILENAME</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Headband Logo Type</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Is Alternate</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Is Home</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Is Team Create Uniform</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Jacket Warmup</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>LOGO_BRAND</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>LOGO_TYPE</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>MyTeam Include</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Number On Shorts</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Override NBA Patch</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Socks Away</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Socks Color N#1</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>Socks Color N#2</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>Socks Color N#3</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>Socks Color N#4</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>Socks Color N#5</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>Socks Home</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>Sponsor Patch</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>TEAM</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>TYPE</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>Uniform Address</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>Uniform File</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>UNIQUEID</t>
         </is>
@@ -591,117 +579,117 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Arm Accessory Color Away</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Arm Accessory Color Home</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Headband Color Away</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Headband Color Home</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Jersey Colors - PRIMARY_COLOR</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Jersey Colors - QUATERNARY_COLOR</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Jersey Colors - QUINTARY_COLOR</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Jersey Colors - TERTIARY_COLOR</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>Leg Accessory Color Away</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Leg Accessory Color Home</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Primary Color Sock</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Quaternary Color Sock</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Quintary Color</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
         <is>
           <t>Quintary Color Sock</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Secondary Color Accessory</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Secondary Color Shoes Color</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Secondary Color Sock</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>Sextary Color</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>Shoe Primary Color Away</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>Sock Color Away</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>Sock Color Home</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Tertiary Color</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>Tertiary Color Sock</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>Under Shirt Color Away</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>Under Shirt Color Home</t>
         </is>

</xml_diff>

<commit_message>
- updated offsets from discobisco for feb 19th update - added discobiscos standalone dynamic base finder (for reference and benchmarking)
</commit_message>
<xml_diff>
--- a/nba2k_editor/Offsets/ImportJerseys.xlsx
+++ b/nba2k_editor/Offsets/ImportJerseys.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,12 +430,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Edition Name</t>
+          <t>EDITION_CRC32B</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>EDITION_CRC32B</t>
+          <t>EDITION_NAME</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -445,27 +445,27 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Headband Logo Type</t>
+          <t>HEADBAND_LOGO_TYPE</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Is Alternate</t>
+          <t>IS_ALTERNATE</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Is Home</t>
+          <t>IS_HOME</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Is Team Create Uniform</t>
+          <t>IS_TEAM_CREATE_UNIFORM</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Jacket Warmup</t>
+          <t>JACKET_WARMUP_CRC32B</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -480,57 +480,57 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>MyTeam Include</t>
+          <t>MYTEAM_INCLUDE</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Number On Shorts</t>
+          <t>NUMBER_ON_SHORTS</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Override NBA Patch</t>
+          <t>OVERRIDE_NBA_PATCH</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Socks Away</t>
+          <t>SOCKS_AWAY</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Socks Color N#1</t>
+          <t>SOCKS_COLOR_N#1</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Socks Color N#2</t>
+          <t>SOCKS_COLOR_N#2</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>Socks Color N#3</t>
+          <t>SOCKS_COLOR_N#3</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>Socks Color N#4</t>
+          <t>SOCKS_COLOR_N#4</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>Socks Color N#5</t>
+          <t>SOCKS_COLOR_N#5</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>Socks Home</t>
+          <t>SOCKS_HOME</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>Sponsor Patch</t>
+          <t>SPONSOR_PATCH</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
@@ -544,16 +544,6 @@
         </is>
       </c>
       <c r="Y1" t="inlineStr">
-        <is>
-          <t>Uniform Address</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>Uniform File</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
         <is>
           <t>UNIQUEID</t>
         </is>
@@ -570,7 +560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,117 +571,137 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Arm Accessory Color Away</t>
+          <t>ARM_ACCESSORY_COLOR_AWAY</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Arm Accessory Color Home</t>
+          <t>ARM_ACCESSORY_COLOR_HOME</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Headband Color Away</t>
+          <t>HEADBAND_COLOR_AWAY</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Headband Color Home</t>
+          <t>HEADBAND_COLOR_HOME</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Jersey Colors - PRIMARY_COLOR</t>
+          <t>LEG_ACCESSORY_COLOR_AWAY</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Jersey Colors - QUATERNARY_COLOR</t>
+          <t>LEG_ACCESSORY_COLOR_HOME</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Jersey Colors - TERTIARY_COLOR</t>
+          <t>PRIMARY_COLOR</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Leg Accessory Color Away</t>
+          <t>PRIMARY_COLOR#ACCESSORY</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Leg Accessory Color Home</t>
+          <t>PRIMARY_COLOR#SOCK</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Primary Color Sock</t>
+          <t>QUATERNARY_COLOR</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Quaternary Color Sock</t>
+          <t>QUATERNARY_COLOR#ACCESSORY</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Quintary Color</t>
+          <t>QUATERNARY_COLOR#SOCK</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Quintary Color Sock</t>
+          <t>QUINTARY_COLOR</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Secondary Color Accessory</t>
+          <t>QUINTARY_COLOR#ACCESSORY</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Secondary Color Shoes Color</t>
+          <t>QUINTARY_COLOR#SOCK</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Secondary Color Sock</t>
+          <t>SECONDARY_COLOR#ACCESSORY</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Sextary Color</t>
+          <t>SECONDARY_COLOR#SOCK</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>Shoe Primary Color Away</t>
+          <t>SECONDARY_COLOR_SHOES_COLOR</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>Sock Color Away</t>
+          <t>SEXTARY_COLOR</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>Sock Color Home</t>
+          <t>SHOE_PRIMARY_COLOR_AWAY</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>Tertiary Color Sock</t>
+          <t>SOCK_COLOR_AWAY</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>Under Shirt Color Away</t>
+          <t>SOCK_COLOR_HOME</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>Under Shirt Color Home</t>
+          <t>TERTIARY_COLOR</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>TERTIARY_COLOR#ACCESSORY</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>TERTIARY_COLOR#SOCK</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>UNDER_SHIRT_COLOR_AWAY</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>UNDER_SHIRT_COLOR_HOME</t>
         </is>
       </c>
     </row>

</xml_diff>